<commit_message>
add coordinate system transforms
</commit_message>
<xml_diff>
--- a/VisualUtilities/Separating Axis Theorem.xlsx
+++ b/VisualUtilities/Separating Axis Theorem.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\ProgrammingUtilities\VisualUtilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2A0FC2-54B9-42B3-8C32-6DE8D05668E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8170206C-79F0-468B-8871-51AE7298347A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8450" yWindow="2150" windowWidth="22230" windowHeight="15370" activeTab="3" xr2:uid="{52B6888F-E73F-4FA9-BE87-9400A268E921}"/>
+    <workbookView xWindow="2230" yWindow="2940" windowWidth="20310" windowHeight="15370" activeTab="3" xr2:uid="{52B6888F-E73F-4FA9-BE87-9400A268E921}"/>
   </bookViews>
   <sheets>
     <sheet name="sat" sheetId="9" r:id="rId1"/>
@@ -295,10 +295,10 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -520,19 +520,19 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>116.94872981077806</c:v>
+                  <c:v>111.69872981077806</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.448729810778062</c:v>
+                  <c:v>61.698729810778062</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>143.05127018922195</c:v>
+                  <c:v>148.30127018922195</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>203.55127018922195</c:v>
+                  <c:v>198.30127018922195</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>116.94872981077806</c:v>
+                  <c:v>111.69872981077806</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,19 +544,19 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>63.105463071041456</c:v>
+                  <c:v>61.698729810778062</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>167.89453692895856</c:v>
+                  <c:v>148.30127018922195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>217.89453692895853</c:v>
+                  <c:v>198.30127018922195</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>113.10546307104146</c:v>
+                  <c:v>111.69872981077806</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63.105463071041456</c:v>
+                  <c:v>61.698729810778062</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2664,10 +2664,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="4" t="s">
@@ -2782,11 +2782,11 @@
       </c>
       <c r="D18" s="6" cm="1">
         <f t="array" ref="D18">IF($B18=1,INDEX(Vertices1,$C18,1),INDEX(Vertices2,$C18,1))</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="E18" s="6" cm="1">
         <f t="array" ref="E18">IF($B18=1,INDEX(Vertices1,$C18,2),INDEX(Vertices2,$C18,2))</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -2800,11 +2800,11 @@
       </c>
       <c r="D19" s="6" cm="1">
         <f t="array" ref="D19">IF($B19=1,INDEX(Vertices1,$C19,1),INDEX(Vertices2,$C19,1))</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="E19" s="6" cm="1">
         <f t="array" ref="E19">IF($B19=1,INDEX(Vertices1,$C19,2),INDEX(Vertices2,$C19,2))</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -2818,11 +2818,11 @@
       </c>
       <c r="D20" s="6" cm="1">
         <f t="array" ref="D20">IF($B20=1,INDEX(Vertices1,$C20,1),INDEX(Vertices2,$C20,1))</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="E20" s="6" cm="1">
         <f t="array" ref="E20">IF($B20=1,INDEX(Vertices1,$C20,2),INDEX(Vertices2,$C20,2))</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -2836,11 +2836,11 @@
       </c>
       <c r="D21" s="6" cm="1">
         <f t="array" ref="D21">IF($B21=1,INDEX(Vertices1,$C21,1),INDEX(Vertices2,$C21,1))</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="E21" s="6" cm="1">
         <f t="array" ref="E21">IF($B21=1,INDEX(Vertices1,$C21,2),INDEX(Vertices2,$C21,2))</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -2853,11 +2853,11 @@
       </c>
       <c r="D22" s="7">
         <f>D18</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="E22" s="7">
         <f>E18</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -2866,23 +2866,23 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
+      <c r="E25" s="9"/>
+      <c r="F25" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8" t="s">
+      <c r="G25" s="9"/>
+      <c r="H25" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="4" t="s">
@@ -2930,11 +2930,11 @@
       </c>
       <c r="F27" s="6">
         <f>_xlfn.MINIFS($I$80:$I$112,$B$80:$B$112,$B27,$C$80:$C$112,$C27)</f>
-        <v>-23283.330249197705</v>
+        <v>-22758.330249197708</v>
       </c>
       <c r="G27" s="6">
         <f>_xlfn.MAXIFS($I$80:$I$112,$B$80:$B$112,$B27,$C$80:$C$112,$C27)</f>
-        <v>-13283.330249197703</v>
+        <v>-12758.330249197703</v>
       </c>
       <c r="H27" t="b">
         <f>AND(D27&lt;G27,D27&gt;F27)</f>
@@ -2968,11 +2968,11 @@
       </c>
       <c r="F28" s="6">
         <f t="shared" ref="F28:F34" si="2">_xlfn.MINIFS($I$80:$I$112,$B$80:$B$112,$B28,$C$80:$C$112,$C28)</f>
-        <v>-382.34307682863619</v>
+        <v>-241.66975080229713</v>
       </c>
       <c r="G28" s="6">
         <f t="shared" ref="G28:G34" si="3">_xlfn.MAXIFS($I$80:$I$112,$B$80:$B$112,$B28,$C$80:$C$112,$C28)</f>
-        <v>11717.656923171367</v>
+        <v>9758.3302491977065</v>
       </c>
       <c r="H28" t="b">
         <f t="shared" ref="H28:H33" si="4">AND(D28&lt;G28,D28&gt;F28)</f>
@@ -3006,11 +3006,11 @@
       </c>
       <c r="F29" s="6">
         <f t="shared" si="2"/>
-        <v>13283.330249197703</v>
+        <v>12758.330249197703</v>
       </c>
       <c r="G29" s="6">
         <f t="shared" si="3"/>
-        <v>23283.330249197705</v>
+        <v>22758.330249197708</v>
       </c>
       <c r="H29" t="b">
         <f t="shared" si="4"/>
@@ -3044,11 +3044,11 @@
       </c>
       <c r="F30" s="6">
         <f t="shared" si="2"/>
-        <v>-11717.656923171367</v>
+        <v>-9758.3302491977065</v>
       </c>
       <c r="G30" s="6">
         <f t="shared" si="3"/>
-        <v>382.34307682863619</v>
+        <v>241.66975080229713</v>
       </c>
       <c r="H30" t="b">
         <f t="shared" si="4"/>
@@ -3074,19 +3074,19 @@
       </c>
       <c r="D31" s="6">
         <f t="shared" si="0"/>
-        <v>-14314.453692895857</v>
+        <v>-11830.127018922196</v>
       </c>
       <c r="E31" s="6">
         <f t="shared" si="1"/>
-        <v>-2214.4536928958532</v>
+        <v>-1830.1270189221927</v>
       </c>
       <c r="F31" s="6">
         <f t="shared" si="2"/>
-        <v>-28172.829601529229</v>
+        <v>-22758.330249197708</v>
       </c>
       <c r="G31" s="6">
         <f t="shared" si="3"/>
-        <v>-16072.829601529222</v>
+        <v>-12758.330249197705</v>
       </c>
       <c r="H31" t="b">
         <f t="shared" si="4"/>
@@ -3112,19 +3112,19 @@
       </c>
       <c r="D32" s="6">
         <f t="shared" si="0"/>
-        <v>-3169.8729810778063</v>
+        <v>-3169.8729810778073</v>
       </c>
       <c r="E32" s="6">
         <f t="shared" si="1"/>
-        <v>6830.1270189221977</v>
+        <v>6830.1270189221959</v>
       </c>
       <c r="F32" s="6">
         <f t="shared" si="2"/>
-        <v>-382.34307682863255</v>
+        <v>-241.66975080229622</v>
       </c>
       <c r="G32" s="6">
         <f t="shared" si="3"/>
-        <v>11717.656923171371</v>
+        <v>9758.3302491977083</v>
       </c>
       <c r="H32" t="b">
         <f t="shared" si="4"/>
@@ -3150,19 +3150,19 @@
       </c>
       <c r="D33" s="6">
         <f t="shared" si="0"/>
-        <v>2214.4536928958523</v>
+        <v>1830.1270189221927</v>
       </c>
       <c r="E33" s="6">
         <f t="shared" si="1"/>
-        <v>14314.453692895855</v>
+        <v>11830.127018922196</v>
       </c>
       <c r="F33" s="6">
         <f t="shared" si="2"/>
-        <v>16072.829601529218</v>
+        <v>12758.330249197705</v>
       </c>
       <c r="G33" s="6">
         <f t="shared" si="3"/>
-        <v>28172.829601529222</v>
+        <v>22758.330249197708</v>
       </c>
       <c r="H33" t="b">
         <f t="shared" si="4"/>
@@ -3196,11 +3196,11 @@
       </c>
       <c r="F34" s="6">
         <f t="shared" si="2"/>
-        <v>-11717.656923171369</v>
+        <v>-9758.3302491977083</v>
       </c>
       <c r="G34" s="6">
         <f t="shared" si="3"/>
-        <v>382.34307682863528</v>
+        <v>241.66975080229622</v>
       </c>
       <c r="H34" t="b">
         <f t="shared" ref="H34" si="7">AND(D34&lt;G34,D34&gt;F34)</f>
@@ -3241,18 +3241,18 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8" t="s">
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="4" t="s">
@@ -3832,11 +3832,11 @@
       </c>
       <c r="D59" s="6" cm="1">
         <f t="array" ref="D59">INDEX(IF($B59=1,Perpendiculars1,Perpendiculars2),$C59,1)</f>
-        <v>-104.7890738579171</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="E59" s="6" cm="1">
         <f t="array" ref="E59">INDEX(IF($B59=1,Perpendiculars1,Perpendiculars2),$C59,2)</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F59">
         <f t="shared" ref="F59:F60" si="22">IF(F58&lt;$B$5,F58+1,1)</f>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="I59" s="6">
         <f t="shared" ref="I59:I60" si="23">SUMPRODUCT($D59:$E59,G59:H59)</f>
-        <v>-2214.4536928958532</v>
+        <v>-1830.1270189221927</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.35">
@@ -3866,11 +3866,11 @@
       </c>
       <c r="D60" s="6" cm="1">
         <f t="array" ref="D60">INDEX(IF($B60=1,Perpendiculars1,Perpendiculars2),$C60,1)</f>
-        <v>-104.7890738579171</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="E60" s="6" cm="1">
         <f t="array" ref="E60">INDEX(IF($B60=1,Perpendiculars1,Perpendiculars2),$C60,2)</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F60">
         <f t="shared" si="22"/>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="I60" s="6">
         <f t="shared" si="23"/>
-        <v>-2214.4536928958532</v>
+        <v>-1830.1270189221927</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.35">
@@ -3900,11 +3900,11 @@
       </c>
       <c r="D61" s="6" cm="1">
         <f t="array" ref="D61">INDEX(IF($B61=1,Perpendiculars1,Perpendiculars2),$C61,1)</f>
-        <v>-104.7890738579171</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="E61" s="6" cm="1">
         <f t="array" ref="E61">INDEX(IF($B61=1,Perpendiculars1,Perpendiculars2),$C61,2)</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F61">
         <f t="shared" ref="F61:F74" si="26">IF(F60&lt;$B$5,F60+1,1)</f>
@@ -3920,7 +3920,7 @@
       </c>
       <c r="I61" s="6">
         <f t="shared" ref="I61:I74" si="27">SUMPRODUCT($D61:$E61,G61:H61)</f>
-        <v>-14314.453692895857</v>
+        <v>-11830.127018922196</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.35">
@@ -3934,11 +3934,11 @@
       </c>
       <c r="D62" s="6" cm="1">
         <f t="array" ref="D62">INDEX(IF($B62=1,Perpendiculars1,Perpendiculars2),$C62,1)</f>
-        <v>-104.7890738579171</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="E62" s="6" cm="1">
         <f t="array" ref="E62">INDEX(IF($B62=1,Perpendiculars1,Perpendiculars2),$C62,2)</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F62">
         <f t="shared" si="26"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="I62" s="6">
         <f t="shared" si="27"/>
-        <v>-14314.453692895857</v>
+        <v>-11830.127018922196</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.35">
@@ -3968,7 +3968,7 @@
       </c>
       <c r="D63" s="6" cm="1">
         <f t="array" ref="D63">INDEX(IF($B63=1,Perpendiculars1,Perpendiculars2),$C63,1)</f>
-        <v>-49.999999999999972</v>
+        <v>-50</v>
       </c>
       <c r="E63" s="6" cm="1">
         <f t="array" ref="E63">INDEX(IF($B63=1,Perpendiculars1,Perpendiculars2),$C63,2)</f>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="I63" s="6">
         <f t="shared" si="27"/>
-        <v>-3169.8729810778063</v>
+        <v>-3169.8729810778073</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.35">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="D64" s="6" cm="1">
         <f t="array" ref="D64">INDEX(IF($B64=1,Perpendiculars1,Perpendiculars2),$C64,1)</f>
-        <v>-49.999999999999972</v>
+        <v>-50</v>
       </c>
       <c r="E64" s="6" cm="1">
         <f t="array" ref="E64">INDEX(IF($B64=1,Perpendiculars1,Perpendiculars2),$C64,2)</f>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="I64" s="6">
         <f t="shared" si="27"/>
-        <v>6830.127018922195</v>
+        <v>6830.1270189221959</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -4036,7 +4036,7 @@
       </c>
       <c r="D65" s="6" cm="1">
         <f t="array" ref="D65">INDEX(IF($B65=1,Perpendiculars1,Perpendiculars2),$C65,1)</f>
-        <v>-49.999999999999972</v>
+        <v>-50</v>
       </c>
       <c r="E65" s="6" cm="1">
         <f t="array" ref="E65">INDEX(IF($B65=1,Perpendiculars1,Perpendiculars2),$C65,2)</f>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="I65" s="6">
         <f t="shared" si="27"/>
-        <v>6830.1270189221977</v>
+        <v>6830.1270189221959</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -4070,7 +4070,7 @@
       </c>
       <c r="D66" s="6" cm="1">
         <f t="array" ref="D66">INDEX(IF($B66=1,Perpendiculars1,Perpendiculars2),$C66,1)</f>
-        <v>-49.999999999999972</v>
+        <v>-50</v>
       </c>
       <c r="E66" s="6" cm="1">
         <f t="array" ref="E66">INDEX(IF($B66=1,Perpendiculars1,Perpendiculars2),$C66,2)</f>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="I66" s="6">
         <f t="shared" si="27"/>
-        <v>-3169.8729810778036</v>
+        <v>-3169.8729810778073</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -4104,11 +4104,11 @@
       </c>
       <c r="D67" s="6" cm="1">
         <f t="array" ref="D67">INDEX(IF($B67=1,Perpendiculars1,Perpendiculars2),$C67,1)</f>
-        <v>104.78907385791707</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="E67" s="6" cm="1">
         <f t="array" ref="E67">INDEX(IF($B67=1,Perpendiculars1,Perpendiculars2),$C67,2)</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F67">
         <f t="shared" si="26"/>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="I67" s="6">
         <f t="shared" si="27"/>
-        <v>2214.4536928958523</v>
+        <v>1830.1270189221927</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="D68" s="6" cm="1">
         <f t="array" ref="D68">INDEX(IF($B68=1,Perpendiculars1,Perpendiculars2),$C68,1)</f>
-        <v>104.78907385791707</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="E68" s="6" cm="1">
         <f t="array" ref="E68">INDEX(IF($B68=1,Perpendiculars1,Perpendiculars2),$C68,2)</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F68">
         <f t="shared" si="26"/>
@@ -4158,7 +4158,7 @@
       </c>
       <c r="I68" s="6">
         <f t="shared" si="27"/>
-        <v>2214.4536928958541</v>
+        <v>1830.1270189221927</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -4172,11 +4172,11 @@
       </c>
       <c r="D69" s="6" cm="1">
         <f t="array" ref="D69">INDEX(IF($B69=1,Perpendiculars1,Perpendiculars2),$C69,1)</f>
-        <v>104.78907385791707</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="E69" s="6" cm="1">
         <f t="array" ref="E69">INDEX(IF($B69=1,Perpendiculars1,Perpendiculars2),$C69,2)</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F69">
         <f t="shared" si="26"/>
@@ -4192,7 +4192,7 @@
       </c>
       <c r="I69" s="6">
         <f t="shared" si="27"/>
-        <v>14314.453692895855</v>
+        <v>11830.127018922196</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -4206,11 +4206,11 @@
       </c>
       <c r="D70" s="6" cm="1">
         <f t="array" ref="D70">INDEX(IF($B70=1,Perpendiculars1,Perpendiculars2),$C70,1)</f>
-        <v>104.78907385791707</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="E70" s="6" cm="1">
         <f t="array" ref="E70">INDEX(IF($B70=1,Perpendiculars1,Perpendiculars2),$C70,2)</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F70">
         <f t="shared" si="26"/>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="I70" s="6">
         <f t="shared" si="27"/>
-        <v>14314.453692895853</v>
+        <v>11830.127018922196</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -4381,18 +4381,18 @@
       </c>
     </row>
     <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B78" s="8" t="s">
+      <c r="B78" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-      <c r="F78" s="8" t="s">
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
-      <c r="I78" s="8"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
     </row>
     <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B79" s="4" t="s">
@@ -4440,15 +4440,15 @@
       </c>
       <c r="G80" s="6" cm="1">
         <f t="array" ref="G80">INDEX(Vertices2,F80,1)</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="H80" s="6" cm="1">
         <f t="array" ref="H80">INDEX(Vertices2,F80,2)</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="I80" s="6">
         <f>SUMPRODUCT($D80:$E80,G80:H80)</f>
-        <v>-13283.330249197703</v>
+        <v>-12758.330249197703</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.35">
@@ -4474,15 +4474,15 @@
       </c>
       <c r="G81" s="6" cm="1">
         <f t="array" ref="G81">INDEX(Vertices2,F81,1)</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="H81" s="6" cm="1">
         <f t="array" ref="H81">INDEX(Vertices2,F81,2)</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="I81" s="6">
         <f t="shared" ref="I81:I97" si="28">SUMPRODUCT($D81:$E81,G81:H81)</f>
-        <v>-13283.330249197703</v>
+        <v>-12758.330249197705</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.35">
@@ -4508,15 +4508,15 @@
       </c>
       <c r="G82" s="6" cm="1">
         <f t="array" ref="G82">INDEX(Vertices2,F82,1)</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="H82" s="6" cm="1">
         <f t="array" ref="H82">INDEX(Vertices2,F82,2)</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="I82" s="6">
         <f t="shared" si="28"/>
-        <v>-23283.330249197705</v>
+        <v>-22758.330249197708</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.35">
@@ -4542,15 +4542,15 @@
       </c>
       <c r="G83" s="6" cm="1">
         <f t="array" ref="G83">INDEX(Vertices2,F83,1)</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="H83" s="6" cm="1">
         <f t="array" ref="H83">INDEX(Vertices2,F83,2)</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="I83" s="6">
         <f t="shared" si="28"/>
-        <v>-23283.330249197705</v>
+        <v>-22758.330249197708</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.35">
@@ -4576,15 +4576,15 @@
       </c>
       <c r="G84" s="6" cm="1">
         <f t="array" ref="G84">INDEX(Vertices2,F84,1)</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="H84" s="6" cm="1">
         <f t="array" ref="H84">INDEX(Vertices2,F84,2)</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="I84" s="6">
         <f t="shared" si="28"/>
-        <v>-382.34307682863619</v>
+        <v>-241.66975080229713</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.35">
@@ -4610,15 +4610,15 @@
       </c>
       <c r="G85" s="6" cm="1">
         <f t="array" ref="G85">INDEX(Vertices2,F85,1)</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="H85" s="6" cm="1">
         <f t="array" ref="H85">INDEX(Vertices2,F85,2)</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="I85" s="6">
         <f t="shared" si="28"/>
-        <v>11717.656923171367</v>
+        <v>9758.3302491977065</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.35">
@@ -4644,15 +4644,15 @@
       </c>
       <c r="G86" s="6" cm="1">
         <f t="array" ref="G86">INDEX(Vertices2,F86,1)</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="H86" s="6" cm="1">
         <f t="array" ref="H86">INDEX(Vertices2,F86,2)</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="I86" s="6">
         <f t="shared" si="28"/>
-        <v>11717.656923171362</v>
+        <v>9758.3302491977047</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.35">
@@ -4678,15 +4678,15 @@
       </c>
       <c r="G87" s="6" cm="1">
         <f t="array" ref="G87">INDEX(Vertices2,F87,1)</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="H87" s="6" cm="1">
         <f t="array" ref="H87">INDEX(Vertices2,F87,2)</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="I87" s="6">
         <f t="shared" si="28"/>
-        <v>-382.34307682863619</v>
+        <v>-241.66975080229713</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.35">
@@ -4712,15 +4712,15 @@
       </c>
       <c r="G88" s="6" cm="1">
         <f t="array" ref="G88">INDEX(Vertices2,F88,1)</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="H88" s="6" cm="1">
         <f t="array" ref="H88">INDEX(Vertices2,F88,2)</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="I88" s="6">
         <f t="shared" si="28"/>
-        <v>13283.330249197703</v>
+        <v>12758.330249197703</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.35">
@@ -4746,15 +4746,15 @@
       </c>
       <c r="G89" s="6" cm="1">
         <f t="array" ref="G89">INDEX(Vertices2,F89,1)</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="H89" s="6" cm="1">
         <f t="array" ref="H89">INDEX(Vertices2,F89,2)</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="I89" s="6">
         <f t="shared" si="28"/>
-        <v>13283.330249197703</v>
+        <v>12758.330249197705</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.35">
@@ -4780,15 +4780,15 @@
       </c>
       <c r="G90" s="6" cm="1">
         <f t="array" ref="G90">INDEX(Vertices2,F90,1)</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="H90" s="6" cm="1">
         <f t="array" ref="H90">INDEX(Vertices2,F90,2)</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="I90" s="6">
         <f t="shared" si="28"/>
-        <v>23283.330249197705</v>
+        <v>22758.330249197708</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.35">
@@ -4814,15 +4814,15 @@
       </c>
       <c r="G91" s="6" cm="1">
         <f t="array" ref="G91">INDEX(Vertices2,F91,1)</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="H91" s="6" cm="1">
         <f t="array" ref="H91">INDEX(Vertices2,F91,2)</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="I91" s="6">
         <f t="shared" si="28"/>
-        <v>23283.330249197705</v>
+        <v>22758.330249197708</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.35">
@@ -4848,15 +4848,15 @@
       </c>
       <c r="G92" s="6" cm="1">
         <f t="array" ref="G92">INDEX(Vertices2,F92,1)</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="H92" s="6" cm="1">
         <f t="array" ref="H92">INDEX(Vertices2,F92,2)</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="I92" s="6">
         <f t="shared" si="28"/>
-        <v>382.34307682863619</v>
+        <v>241.66975080229713</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.35">
@@ -4882,15 +4882,15 @@
       </c>
       <c r="G93" s="6" cm="1">
         <f t="array" ref="G93">INDEX(Vertices2,F93,1)</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="H93" s="6" cm="1">
         <f t="array" ref="H93">INDEX(Vertices2,F93,2)</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="I93" s="6">
         <f t="shared" si="28"/>
-        <v>-11717.656923171367</v>
+        <v>-9758.3302491977065</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.35">
@@ -4916,15 +4916,15 @@
       </c>
       <c r="G94" s="6" cm="1">
         <f t="array" ref="G94">INDEX(Vertices2,F94,1)</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="H94" s="6" cm="1">
         <f t="array" ref="H94">INDEX(Vertices2,F94,2)</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="I94" s="6">
         <f t="shared" si="28"/>
-        <v>-11717.656923171362</v>
+        <v>-9758.3302491977047</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.35">
@@ -4950,15 +4950,15 @@
       </c>
       <c r="G95" s="6" cm="1">
         <f t="array" ref="G95">INDEX(Vertices2,F95,1)</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="H95" s="6" cm="1">
         <f t="array" ref="H95">INDEX(Vertices2,F95,2)</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="I95" s="6">
         <f t="shared" si="28"/>
-        <v>382.34307682863619</v>
+        <v>241.66975080229713</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.35">
@@ -4972,11 +4972,11 @@
       </c>
       <c r="D96" s="6" cm="1">
         <f t="array" ref="D96">INDEX(IF($B96=1,Perpendiculars1,Perpendiculars2),$C96,1)</f>
-        <v>-104.7890738579171</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="E96" s="6" cm="1">
         <f t="array" ref="E96">INDEX(IF($B96=1,Perpendiculars1,Perpendiculars2),$C96,2)</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F96">
         <f t="shared" si="31"/>
@@ -4984,15 +4984,15 @@
       </c>
       <c r="G96" s="6" cm="1">
         <f t="array" ref="G96">INDEX(Vertices2,F96,1)</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="H96" s="6" cm="1">
         <f t="array" ref="H96">INDEX(Vertices2,F96,2)</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="I96" s="6">
         <f t="shared" si="28"/>
-        <v>-16072.829601529222</v>
+        <v>-12758.330249197705</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.35">
@@ -5006,11 +5006,11 @@
       </c>
       <c r="D97" s="6" cm="1">
         <f t="array" ref="D97">INDEX(IF($B97=1,Perpendiculars1,Perpendiculars2),$C97,1)</f>
-        <v>-104.7890738579171</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="E97" s="6" cm="1">
         <f t="array" ref="E97">INDEX(IF($B97=1,Perpendiculars1,Perpendiculars2),$C97,2)</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F97">
         <f t="shared" si="31"/>
@@ -5018,15 +5018,15 @@
       </c>
       <c r="G97" s="6" cm="1">
         <f t="array" ref="G97">INDEX(Vertices2,F97,1)</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="H97" s="6" cm="1">
         <f t="array" ref="H97">INDEX(Vertices2,F97,2)</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="I97" s="6">
         <f t="shared" si="28"/>
-        <v>-16072.829601529222</v>
+        <v>-12758.330249197705</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.35">
@@ -5040,11 +5040,11 @@
       </c>
       <c r="D98" s="6" cm="1">
         <f t="array" ref="D98">INDEX(IF($B98=1,Perpendiculars1,Perpendiculars2),$C98,1)</f>
-        <v>-104.7890738579171</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="E98" s="6" cm="1">
         <f t="array" ref="E98">INDEX(IF($B98=1,Perpendiculars1,Perpendiculars2),$C98,2)</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F98">
         <f t="shared" ref="F98:F108" si="34">IF(F97&lt;$B$5,F97+1,1)</f>
@@ -5052,15 +5052,15 @@
       </c>
       <c r="G98" s="6" cm="1">
         <f t="array" ref="G98">INDEX(Vertices2,F98,1)</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="H98" s="6" cm="1">
         <f t="array" ref="H98">INDEX(Vertices2,F98,2)</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="I98" s="6">
         <f t="shared" ref="I98:I108" si="35">SUMPRODUCT($D98:$E98,G98:H98)</f>
-        <v>-28172.829601529225</v>
+        <v>-22758.330249197708</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.35">
@@ -5074,11 +5074,11 @@
       </c>
       <c r="D99" s="6" cm="1">
         <f t="array" ref="D99">INDEX(IF($B99=1,Perpendiculars1,Perpendiculars2),$C99,1)</f>
-        <v>-104.7890738579171</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="E99" s="6" cm="1">
         <f t="array" ref="E99">INDEX(IF($B99=1,Perpendiculars1,Perpendiculars2),$C99,2)</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F99">
         <f t="shared" si="34"/>
@@ -5086,15 +5086,15 @@
       </c>
       <c r="G99" s="6" cm="1">
         <f t="array" ref="G99">INDEX(Vertices2,F99,1)</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="H99" s="6" cm="1">
         <f t="array" ref="H99">INDEX(Vertices2,F99,2)</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="I99" s="6">
         <f t="shared" si="35"/>
-        <v>-28172.829601529229</v>
+        <v>-22758.330249197708</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.35">
@@ -5108,7 +5108,7 @@
       </c>
       <c r="D100" s="6" cm="1">
         <f t="array" ref="D100">INDEX(IF($B100=1,Perpendiculars1,Perpendiculars2),$C100,1)</f>
-        <v>-49.999999999999972</v>
+        <v>-50</v>
       </c>
       <c r="E100" s="6" cm="1">
         <f t="array" ref="E100">INDEX(IF($B100=1,Perpendiculars1,Perpendiculars2),$C100,2)</f>
@@ -5120,15 +5120,15 @@
       </c>
       <c r="G100" s="6" cm="1">
         <f t="array" ref="G100">INDEX(Vertices2,F100,1)</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="H100" s="6" cm="1">
         <f t="array" ref="H100">INDEX(Vertices2,F100,2)</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="I100" s="6">
         <f t="shared" si="35"/>
-        <v>-382.34307682863255</v>
+        <v>-241.66975080229622</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.35">
@@ -5142,7 +5142,7 @@
       </c>
       <c r="D101" s="6" cm="1">
         <f t="array" ref="D101">INDEX(IF($B101=1,Perpendiculars1,Perpendiculars2),$C101,1)</f>
-        <v>-49.999999999999972</v>
+        <v>-50</v>
       </c>
       <c r="E101" s="6" cm="1">
         <f t="array" ref="E101">INDEX(IF($B101=1,Perpendiculars1,Perpendiculars2),$C101,2)</f>
@@ -5154,15 +5154,15 @@
       </c>
       <c r="G101" s="6" cm="1">
         <f t="array" ref="G101">INDEX(Vertices2,F101,1)</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="H101" s="6" cm="1">
         <f t="array" ref="H101">INDEX(Vertices2,F101,2)</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="I101" s="6">
         <f t="shared" si="35"/>
-        <v>11717.656923171371</v>
+        <v>9758.3302491977083</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.35">
@@ -5176,7 +5176,7 @@
       </c>
       <c r="D102" s="6" cm="1">
         <f t="array" ref="D102">INDEX(IF($B102=1,Perpendiculars1,Perpendiculars2),$C102,1)</f>
-        <v>-49.999999999999972</v>
+        <v>-50</v>
       </c>
       <c r="E102" s="6" cm="1">
         <f t="array" ref="E102">INDEX(IF($B102=1,Perpendiculars1,Perpendiculars2),$C102,2)</f>
@@ -5188,15 +5188,15 @@
       </c>
       <c r="G102" s="6" cm="1">
         <f t="array" ref="G102">INDEX(Vertices2,F102,1)</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="H102" s="6" cm="1">
         <f t="array" ref="H102">INDEX(Vertices2,F102,2)</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="I102" s="6">
         <f t="shared" si="35"/>
-        <v>11717.656923171371</v>
+        <v>9758.3302491977083</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.35">
@@ -5210,7 +5210,7 @@
       </c>
       <c r="D103" s="6" cm="1">
         <f t="array" ref="D103">INDEX(IF($B103=1,Perpendiculars1,Perpendiculars2),$C103,1)</f>
-        <v>-49.999999999999972</v>
+        <v>-50</v>
       </c>
       <c r="E103" s="6" cm="1">
         <f t="array" ref="E103">INDEX(IF($B103=1,Perpendiculars1,Perpendiculars2),$C103,2)</f>
@@ -5222,15 +5222,15 @@
       </c>
       <c r="G103" s="6" cm="1">
         <f t="array" ref="G103">INDEX(Vertices2,F103,1)</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="H103" s="6" cm="1">
         <f t="array" ref="H103">INDEX(Vertices2,F103,2)</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="I103" s="6">
         <f t="shared" si="35"/>
-        <v>-382.34307682862891</v>
+        <v>-241.66975080229531</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.35">
@@ -5244,11 +5244,11 @@
       </c>
       <c r="D104" s="6" cm="1">
         <f t="array" ref="D104">INDEX(IF($B104=1,Perpendiculars1,Perpendiculars2),$C104,1)</f>
-        <v>104.78907385791707</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="E104" s="6" cm="1">
         <f t="array" ref="E104">INDEX(IF($B104=1,Perpendiculars1,Perpendiculars2),$C104,2)</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F104">
         <f t="shared" si="34"/>
@@ -5256,15 +5256,15 @@
       </c>
       <c r="G104" s="6" cm="1">
         <f t="array" ref="G104">INDEX(Vertices2,F104,1)</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="H104" s="6" cm="1">
         <f t="array" ref="H104">INDEX(Vertices2,F104,2)</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="I104" s="6">
         <f t="shared" si="35"/>
-        <v>16072.829601529218</v>
+        <v>12758.330249197705</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.35">
@@ -5278,11 +5278,11 @@
       </c>
       <c r="D105" s="6" cm="1">
         <f t="array" ref="D105">INDEX(IF($B105=1,Perpendiculars1,Perpendiculars2),$C105,1)</f>
-        <v>104.78907385791707</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="E105" s="6" cm="1">
         <f t="array" ref="E105">INDEX(IF($B105=1,Perpendiculars1,Perpendiculars2),$C105,2)</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F105">
         <f t="shared" si="34"/>
@@ -5290,15 +5290,15 @@
       </c>
       <c r="G105" s="6" cm="1">
         <f t="array" ref="G105">INDEX(Vertices2,F105,1)</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="H105" s="6" cm="1">
         <f t="array" ref="H105">INDEX(Vertices2,F105,2)</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="I105" s="6">
         <f t="shared" si="35"/>
-        <v>16072.82960152922</v>
+        <v>12758.330249197705</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.35">
@@ -5312,11 +5312,11 @@
       </c>
       <c r="D106" s="6" cm="1">
         <f t="array" ref="D106">INDEX(IF($B106=1,Perpendiculars1,Perpendiculars2),$C106,1)</f>
-        <v>104.78907385791707</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="E106" s="6" cm="1">
         <f t="array" ref="E106">INDEX(IF($B106=1,Perpendiculars1,Perpendiculars2),$C106,2)</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F106">
         <f t="shared" si="34"/>
@@ -5324,15 +5324,15 @@
       </c>
       <c r="G106" s="6" cm="1">
         <f t="array" ref="G106">INDEX(Vertices2,F106,1)</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="H106" s="6" cm="1">
         <f t="array" ref="H106">INDEX(Vertices2,F106,2)</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="I106" s="6">
         <f t="shared" si="35"/>
-        <v>28172.829601529222</v>
+        <v>22758.330249197708</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.35">
@@ -5346,11 +5346,11 @@
       </c>
       <c r="D107" s="6" cm="1">
         <f t="array" ref="D107">INDEX(IF($B107=1,Perpendiculars1,Perpendiculars2),$C107,1)</f>
-        <v>104.78907385791707</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="E107" s="6" cm="1">
         <f t="array" ref="E107">INDEX(IF($B107=1,Perpendiculars1,Perpendiculars2),$C107,2)</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F107">
         <f t="shared" si="34"/>
@@ -5358,15 +5358,15 @@
       </c>
       <c r="G107" s="6" cm="1">
         <f t="array" ref="G107">INDEX(Vertices2,F107,1)</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="H107" s="6" cm="1">
         <f t="array" ref="H107">INDEX(Vertices2,F107,2)</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="I107" s="6">
         <f t="shared" si="35"/>
-        <v>28172.829601529222</v>
+        <v>22758.330249197708</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.35">
@@ -5392,15 +5392,15 @@
       </c>
       <c r="G108" s="6" cm="1">
         <f t="array" ref="G108">INDEX(Vertices2,F108,1)</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="H108" s="6" cm="1">
         <f t="array" ref="H108">INDEX(Vertices2,F108,2)</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="I108" s="6">
         <f t="shared" si="35"/>
-        <v>382.34307682863528</v>
+        <v>241.66975080229622</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.35">
@@ -5426,15 +5426,15 @@
       </c>
       <c r="G109" s="6" cm="1">
         <f t="array" ref="G109">INDEX(Vertices2,F109,1)</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="H109" s="6" cm="1">
         <f t="array" ref="H109">INDEX(Vertices2,F109,2)</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="I109" s="6">
         <f t="shared" ref="I109:I111" si="39">SUMPRODUCT($D109:$E109,G109:H109)</f>
-        <v>-11717.656923171369</v>
+        <v>-9758.3302491977083</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.35">
@@ -5460,15 +5460,15 @@
       </c>
       <c r="G110" s="6" cm="1">
         <f t="array" ref="G110">INDEX(Vertices2,F110,1)</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="H110" s="6" cm="1">
         <f t="array" ref="H110">INDEX(Vertices2,F110,2)</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="I110" s="6">
         <f t="shared" si="39"/>
-        <v>-11717.656923171366</v>
+        <v>-9758.3302491977083</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.35">
@@ -5494,15 +5494,15 @@
       </c>
       <c r="G111" s="6" cm="1">
         <f t="array" ref="G111">INDEX(Vertices2,F111,1)</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="H111" s="6" cm="1">
         <f t="array" ref="H111">INDEX(Vertices2,F111,2)</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="I111" s="6">
         <f t="shared" si="39"/>
-        <v>382.34307682863437</v>
+        <v>241.66975080229531</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.35">
@@ -5630,52 +5630,52 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8" t="s">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8" t="s">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="8"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8" t="s">
+      <c r="I11" s="9"/>
+      <c r="J11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8" t="s">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="8"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
@@ -6055,10 +6055,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4342B3CF-D73B-451F-BB44-4AFED380BCFB}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6108,52 +6108,52 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8" t="s">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8" t="s">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="8"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8" t="s">
+      <c r="I11" s="9"/>
+      <c r="J11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8" t="s">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="8"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
@@ -6212,39 +6212,39 @@
       </c>
       <c r="E13">
         <f>C13-$C$21</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F13">
         <f>D13*COS($C$6)-E13*SIN($C$6)</f>
-        <v>-13.051270189221942</v>
+        <v>-18.301270189221942</v>
       </c>
       <c r="G13">
         <f>D13*SIN($C$6)+E13*COS($C$6)</f>
-        <v>-77.394536928958544</v>
+        <v>-68.301270189221938</v>
       </c>
       <c r="H13">
         <f>F13+$B$21</f>
-        <v>116.94872981077806</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="I13">
         <f>G13+$C$21</f>
-        <v>63.105463071041456</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="J13" cm="1">
         <f t="array" ref="J13">IF($A13&lt;$B$8,INDEX(Vertices2,$A13+1,1),INDEX(Vertices2,1,1))-INDEX(Vertices2,$A13,1)</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="K13" cm="1">
         <f t="array" ref="K13">IF($A13&lt;$B$8,INDEX(Vertices2,$A13+1,2),INDEX(Vertices2,1,2))-INDEX(Vertices2,$A13,2)</f>
-        <v>104.7890738579171</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="L13">
         <f>-K13</f>
-        <v>-104.7890738579171</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="M13">
         <f>J13</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -6256,7 +6256,7 @@
         <v>80</v>
       </c>
       <c r="C14">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="D14">
         <f>B14-$B$21</f>
@@ -6264,23 +6264,23 @@
       </c>
       <c r="E14">
         <f>C14-$C$21</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F14">
         <f>D14*COS($C$6)-E14*SIN($C$6)</f>
-        <v>-73.551270189221938</v>
+        <v>-68.301270189221938</v>
       </c>
       <c r="G14">
         <f>D14*SIN($C$6)+E14*COS($C$6)</f>
-        <v>27.394536928958548</v>
+        <v>18.301270189221942</v>
       </c>
       <c r="H14">
         <f>F14+$B$21</f>
-        <v>56.448729810778062</v>
+        <v>61.698729810778062</v>
       </c>
       <c r="I14">
         <f>G14+$C$21</f>
-        <v>167.89453692895856</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="J14" cm="1">
         <f t="array" ref="J14">IF($A14&lt;$B$8,INDEX(Vertices2,$A14+1,1),INDEX(Vertices2,1,1))-INDEX(Vertices2,$A14,1)</f>
@@ -6288,11 +6288,11 @@
       </c>
       <c r="K14" cm="1">
         <f t="array" ref="K14">IF($A14&lt;$B$8,INDEX(Vertices2,$A14+1,2),INDEX(Vertices2,1,2))-INDEX(Vertices2,$A14,2)</f>
-        <v>49.999999999999972</v>
+        <v>50</v>
       </c>
       <c r="L14">
         <f t="shared" ref="L14:L16" si="0">-K14</f>
-        <v>-49.999999999999972</v>
+        <v>-50</v>
       </c>
       <c r="M14">
         <f t="shared" ref="M14:M16" si="1">J14</f>
@@ -6308,7 +6308,7 @@
         <v>180</v>
       </c>
       <c r="C15">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="D15">
         <f>B15-$B$21</f>
@@ -6316,39 +6316,39 @@
       </c>
       <c r="E15">
         <f>C15-$C$21</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="F15">
         <f>D15*COS($C$6)-E15*SIN($C$6)</f>
-        <v>13.051270189221942</v>
+        <v>18.301270189221942</v>
       </c>
       <c r="G15">
         <f>D15*SIN($C$6)+E15*COS($C$6)</f>
-        <v>77.394536928958544</v>
+        <v>68.301270189221938</v>
       </c>
       <c r="H15">
         <f>F15+$B$21</f>
-        <v>143.05127018922195</v>
+        <v>148.30127018922195</v>
       </c>
       <c r="I15">
         <f>G15+$C$21</f>
-        <v>217.89453692895853</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="J15" cm="1">
         <f t="array" ref="J15">IF($A15&lt;$B$8,INDEX(Vertices2,$A15+1,1),INDEX(Vertices2,1,1))-INDEX(Vertices2,$A15,1)</f>
-        <v>60.5</v>
+        <v>50</v>
       </c>
       <c r="K15" cm="1">
         <f t="array" ref="K15">IF($A15&lt;$B$8,INDEX(Vertices2,$A15+1,2),INDEX(Vertices2,1,2))-INDEX(Vertices2,$A15,2)</f>
-        <v>-104.78907385791707</v>
+        <v>-86.602540378443891</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>104.78907385791707</v>
+        <v>86.602540378443891</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>60.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -6368,23 +6368,23 @@
       </c>
       <c r="E16">
         <f>C16-$C$21</f>
-        <v>-60.5</v>
+        <v>-50</v>
       </c>
       <c r="F16">
         <f>D16*COS($C$6)-E16*SIN($C$6)</f>
-        <v>73.551270189221938</v>
+        <v>68.301270189221938</v>
       </c>
       <c r="G16">
         <f>D16*SIN($C$6)+E16*COS($C$6)</f>
-        <v>-27.394536928958548</v>
+        <v>-18.301270189221942</v>
       </c>
       <c r="H16">
         <f>F16+$B$21</f>
-        <v>203.55127018922195</v>
+        <v>198.30127018922195</v>
       </c>
       <c r="I16">
         <f>G16+$C$21</f>
-        <v>113.10546307104146</v>
+        <v>111.69872981077806</v>
       </c>
       <c r="J16" cm="1">
         <f t="array" ref="J16">IF($A16&lt;$B$8,INDEX(Vertices2,$A16+1,1),INDEX(Vertices2,1,1))-INDEX(Vertices2,$A16,1)</f>
@@ -6441,7 +6441,7 @@
       </c>
       <c r="C21">
         <f>AVERAGE(C13:C17)</f>
-        <v>140.5</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
@@ -6474,6 +6474,38 @@
       </c>
       <c r="C28">
         <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>80</v>
+      </c>
+      <c r="C32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>80</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -6518,14 +6550,14 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
@@ -6580,52 +6612,52 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8" t="s">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8" t="s">
+      <c r="I12" s="9"/>
+      <c r="J12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
+      <c r="G13" s="9"/>
+      <c r="H13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8" t="s">
+      <c r="I13" s="9"/>
+      <c r="J13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8" t="s">
+      <c r="K13" s="9"/>
+      <c r="L13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="8"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
@@ -6952,11 +6984,11 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B29">
-        <f>B15</f>
+        <f t="shared" ref="B29:C32" si="11">B15</f>
         <v>80</v>
       </c>
       <c r="C29">
-        <f>C15</f>
+        <f t="shared" si="11"/>
         <v>80</v>
       </c>
       <c r="D29">
@@ -6970,55 +7002,55 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B30">
-        <f>B16</f>
+        <f t="shared" si="11"/>
         <v>80</v>
       </c>
       <c r="C30">
-        <f>C16</f>
+        <f t="shared" si="11"/>
         <v>201</v>
       </c>
       <c r="D30">
-        <f t="shared" ref="D30:E30" si="11">L16</f>
+        <f t="shared" ref="D30:E30" si="12">L16</f>
         <v>158.97441116742348</v>
       </c>
       <c r="E30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>104.26348502534057</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B31">
-        <f>B17</f>
+        <f t="shared" si="11"/>
         <v>180</v>
       </c>
       <c r="C31">
-        <f>C17</f>
+        <f t="shared" si="11"/>
         <v>201</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:E31" si="12">L17</f>
+        <f t="shared" ref="D31:E31" si="13">L17</f>
         <v>245.57695154586736</v>
       </c>
       <c r="E31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>154.26348502534057</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B32">
-        <f>B18</f>
+        <f t="shared" si="11"/>
         <v>180</v>
       </c>
       <c r="C32">
-        <f>C18</f>
+        <f t="shared" si="11"/>
         <v>80</v>
       </c>
       <c r="D32">
-        <f t="shared" ref="D32:E32" si="13">L18</f>
+        <f t="shared" ref="D32:E32" si="14">L18</f>
         <v>306.07695154586736</v>
       </c>
       <c r="E32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>49.474411167423483</v>
       </c>
     </row>
@@ -7028,15 +7060,15 @@
         <v>80</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" ref="C33:E33" si="14">C29</f>
+        <f t="shared" ref="C33:E33" si="15">C29</f>
         <v>80</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>219.47441116742345</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.52558883257648858</v>
       </c>
     </row>

</xml_diff>